<commit_message>
Node and Html dashboard code
</commit_message>
<xml_diff>
--- a/links.xlsx
+++ b/links.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>https://github.com/</t>
   </si>
@@ -32,16 +32,30 @@
   </si>
   <si>
     <t>https://www.microsoft.com/en-in</t>
+  </si>
+  <si>
+    <t>https://esign.verasys.in/</t>
+  </si>
+  <si>
+    <t>https://vsign.in/</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -64,13 +78,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -373,13 +390,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A6"/>
+  <dimension ref="A1:A8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="32.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -411,7 +431,21 @@
         <v>5</v>
       </c>
     </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A7" r:id="rId1"/>
+    <hyperlink ref="A8" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>